<commit_message>
login done (save info big delay bug)
</commit_message>
<xml_diff>
--- a/LogInCredentials.xlsx
+++ b/LogInCredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\AN_3\SEM_1\RPA\RPA-Project\RPA-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B6D05A-5657-43CB-B867-F7A13ED46557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F8F957-D842-4933-B34B-215F251990F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>rpapassword123</t>
+    <t>rpatestacc@gmail.com</t>
   </si>
   <si>
-    <t>rpatestacc@gmail.com</t>
+    <t>rpapassword123</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,10 +387,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Followers scraping (bug when few followers)
</commit_message>
<xml_diff>
--- a/LogInCredentials.xlsx
+++ b/LogInCredentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\AN_3\SEM_1\RPA\RPA-Project\RPA-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F8F957-D842-4933-B34B-215F251990F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1813953-392B-488B-A1C5-0B47F034E672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>rpatestacc@gmail.com</t>
+    <t>rpapassword123</t>
   </si>
   <si>
-    <t>rpapassword123</t>
+    <t>rpatestacc</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,15 +387,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{2C0DBC66-9600-49A7-A171-7B085FEE83BC}"/>
+    <hyperlink ref="A2" r:id="rId1" display="rpatestacc@gmail.com" xr:uid="{2C0DBC66-9600-49A7-A171-7B085FEE83BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>